<commit_message>
Add test case for classification
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27907"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MasterAu/Documents/GitHub/team-capers/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylandecker/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24CA8C7-F859-1144-BE69-5B500FCFE899}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{F0D21C0D-FC9E-ED4F-BBF9-4AB2B50626E6}"/>
+    <workbookView xWindow="4420" yWindow="1020" windowWidth="25600" windowHeight="14640"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>INPUT</t>
   </si>
@@ -141,12 +146,24 @@
   </si>
   <si>
     <t>Invalid entry end date is before start date</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Classification</t>
+  </si>
+  <si>
+    <t>Choose the 'private' option</t>
+  </si>
+  <si>
+    <t>Your .ics will be created with a "private" visibility setting.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -500,11 +517,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA4AE9EE-7BD7-FC43-8B52-33FEFC537E83}">
-  <dimension ref="A1:C12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -646,6 +663,22 @@
         <v>35</v>
       </c>
     </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>